<commit_message>
About to Switch to Ingrediant Based Recipes
</commit_message>
<xml_diff>
--- a/ItemCrafting/Magic_Wepon_effects.xlsx
+++ b/ItemCrafting/Magic_Wepon_effects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\ItemCrafting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC69625E-774F-45BD-A644-CEF289F6CA7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2FCB36-2D9F-4A7E-B4DB-CDFE97BF558E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1060,8 +1060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>